<commit_message>
Update template FAQ to clarify affiliations sheet
</commit_message>
<xml_diff>
--- a/metrics/config/template.xlsx
+++ b/metrics/config/template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Documents/application/Dataverse_Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/Dataverse-Report/metrics/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1A571E-A257-574C-BB4C-5F6A69538580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="11980"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="16320" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Tab</t>
   </si>
@@ -86,9 +87,6 @@
     <t>Totals</t>
   </si>
   <si>
-    <t>The number of users by affiliation over the one year time period</t>
-  </si>
-  <si>
     <t>All time</t>
   </si>
   <si>
@@ -126,12 +124,21 @@
   </si>
   <si>
     <t>FAQ</t>
+  </si>
+  <si>
+    <t>The number of new users by affiliation over the one year time period</t>
+  </si>
+  <si>
+    <t>Month - Year</t>
+  </si>
+  <si>
+    <t>The number of new users by affiliation over the month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -604,11 +611,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -620,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -640,7 +647,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -667,7 +674,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -676,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -694,7 +701,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -717,20 +724,20 @@
     </row>
     <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,7 +746,7 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -748,25 +755,34 @@
         <v>16</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>